<commit_message>
updated xls data file
</commit_message>
<xml_diff>
--- a/src/test/resources/data/GitHubRepoList.xlsx
+++ b/src/test/resources/data/GitHubRepoList.xlsx
@@ -25,7 +25,7 @@
     <t>private</t>
   </si>
   <si>
-    <t xml:space="preserve"> GitHubHandling_UsingRestAssured</t>
+    <t xml:space="preserve"> GitHubSampleRepo1</t>
   </si>
   <si>
     <t>creating,updating,deleting Repos.
@@ -36,25 +36,25 @@
     <t>http://github.com</t>
   </si>
   <si>
-    <t>Guru99DemoPOM</t>
+    <t>GitHubSampleRepo2</t>
   </si>
   <si>
     <t>created selenium automation project using Page Object Model</t>
   </si>
   <si>
-    <t>RestAPIAutomationUsingHttpClients</t>
+    <t>GitHubSampleRepo3</t>
   </si>
   <si>
     <t>Automated RestAPI using HttpClients</t>
   </si>
   <si>
-    <t>SeleniumBasicsProject</t>
+    <t xml:space="preserve"> GitHubSampleRepo4</t>
   </si>
   <si>
     <t>all selenium basics:locators,frames,popups</t>
   </si>
   <si>
-    <t>TestNGProject</t>
+    <t>GitHubSampleRepo5</t>
   </si>
   <si>
     <t>covers all TestNG basics:annotations,data providers,extent reports,listeners</t>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -86,8 +86,12 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +104,12 @@
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -107,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -120,6 +130,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,7 +406,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -407,7 +420,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -435,7 +448,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">

</xml_diff>